<commit_message>
updating datasets for restigouche RST data in order to exclude all sites that are not from `Kedgwick-RST`; removing geojson files (part II)
</commit_message>
<xml_diff>
--- a/17bda544 (restigouche RST)/rst_data_dictionary.xlsx
+++ b/17bda544 (restigouche RST)/rst_data_dictionary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="89">
   <si>
     <t>Data Dictionary - dictionnaire des données</t>
   </si>
@@ -22,6 +22,9 @@
     <t>NAME__NOM</t>
   </si>
   <si>
+    <t>DOCUMENT</t>
+  </si>
+  <si>
     <t>DESCRIPTION_EN</t>
   </si>
   <si>
@@ -29,6 +32,9 @@
   </si>
   <si>
     <t>river_name__nom_de_la_rivière</t>
+  </si>
+  <si>
+    <t>dataset</t>
   </si>
   <si>
     <t>Name of the river</t>
@@ -163,36 +169,44 @@
     <t>status__statut</t>
   </si>
   <si>
-    <t xml:space="preserve">Mortality: Dead fish
-Mortality, recapture: Dead fish; previously sampled (indicated by presence of tag, fin clip, etc.)
-Mortality, research removal: Fish captured alive; kept for research purposes
-Mortality, sampled: Dead fish; biological details collected
-Mortality, tagging: Dead fish as a result of the tagging process.
-Released, injury: Fish captured, released; no biological details recorded due to existing injury
-Released, lost: Fish captured; escaped before biological details recorded
-Released, recaptured: Fish recaptured, released; presence of tag/marking 
-Released, recaptured, lost: Fish recaptured; presence of tag/marking; escaped
-Released, sampled: Fish captured, released; biological details recorded
-Released, tagged: Fish captured, released; biological details recorded, fish tagged
-Released, unsampled: Fish captured, released; no biological details recorded
-Scarred, tag lost, released: Fish recaptured, released; presence of tag/marking
-Unknown	</t>
-  </si>
-  <si>
-    <t>Mortalité: Poisson mort
-Mortalité, recapture: Poisson mort ; échantillonné précédemment (indiqué par la présence d'une étiquette, d'une entaille sur la nageoire, etc.)
-Mortalité, prélèvement à des fins de recherche: Poisson capturé vivant ; conservé à des fins de recherche
-Mortalité, échantillonné: Poisson mort ; détails biologiques collectés
-Mortalité, marqué : Poisson mort à la suite du processus de marquage.
-Remis à l'eau, blessé: Poisson capturé, remis à l'eau ; aucun détail biologique enregistré en raison d'une blessure existante
-Remis à l'eau, perdu: Poisson capturé ; s'est échappé avant que les données biologiques ne soient enregistrées
-Relâché, recapturé: Poisson recapturé, relâché ; présence d'une étiquette/marquage 
-Remis à l'eau, recapturé, perdu: Poisson recapturé ; présence d'une étiquette/marquage ; échappé
-Remis à l'eau, échantillonné: Poisson capturé, remis à l'eau ; détails biologiques enregistrés
-Remis à l'eau, marqué: Poisson capturé, remis à l'eau ; détails biologiques enregistrés, poisson marqué
-Remis à l'eau, non échantillonné: Poisson capturé, remis à l'eau ; aucun détail biologique enregistré
-Cicatrice, étiquette perdue, remis à l'eau : Poisson recapturé, relâché ; présence d'une étiquette/marquage
-Inconnu</t>
+    <t xml:space="preserve">Euthanized: Specimen was euthanized for reasons other than research removal. For example, euthanized because it is an invasive species.
+Mortality: Dead fish.
+Mortality, lost: Deceased specimen that is lost before biological details are recorded.
+Mortality, recapture (and sampled): Dead fish previously sampled (indicated by presence of tag, fin clip, etc.)
+Mortality, sampled: Dead fish, biological details recorded.
+Mortality, tagging: Fish died as a result of the tagging process.
+Mortality, research removal: Fish captured alive and kept for research purposes (fish euthanized).
+Released, unsampled: Fish captured and released: no biological details recorded.
+Released, internal acoustic tag: Specimen captured and released; biological details recorded and fish tagged with an internal acoustic tag.
+Released, injured: Fish captured and released: no biological details recorded due to existing injury.
+Released, lost: Fish captured, but escaped before biological details recorded.
+Released, recaptured: Fish recaptured and released: presence of tag/marking.
+Released, recaptured, lost: Fish recaptured: presence of tag/marking, escaped.
+Released, sampled: Fish captured and released: biological details recorded.
+Released, tagged (and sampled): Fish captured and released; biological details were recorded and fish was tagged.
+Scarred, tag lost, released: Fish recaptured and released: presence of scarring indicates the fish was previously tagged/ marked; tag was lost.
+Unknown: 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None: 
+Mortalité: Poisson mort.
+Mortalité, perdu: Spécimen décédé qui est perdu avant que les détails biologiques ne soient enregistrés.
+Mortalité, recapture (et échantillonné): Poisson mort échantillonné précédemment (indiqué par la présence d'une étiquette, d'une entaille sur la nageoire, etc.).
+Mortalité, échantillonné: Poisson mort, détails biologiques enregistrés.
+Mortalité, marqué: Poisson mort à la suite du processus de marquage.
+Mortalité, prélèvement à des fins de recherche: Poisson capturé vivant et conservé à des fins de recherche (poisson euthanasié).
+Remis à l'eau, non échantillonné: Poisson capturé et remis à l'eau: aucun détail biologique enregistré.
+Remis à l'eau, étiquette acoustique interne: Le spécimen a été capturé et relâché ; les détails biologiques ont été enregistrés et le poisson a été marqué avec une balise acoustique interne.
+Remis à l'eau, blessé: Poisson capturé et remis à l'eau: aucun détail biologique enregistré en raison d'une blessure existante.
+Remis à l'eau, perdu: Poisson capturé, mais qui a réussi à s'échapper avant que les données biologiques ne soient enregistrées.
+Remis à l'eau, recapturé: Poisson recapturé et relâché : présence d'une étiquette/marquage.
+Remis à l'eau, recapturé, perdu: Poisson recapturé ; présence d'une étiquette/marquage, s'est échappé.
+Remis à l'eau, échantillonné: Poisson capturé et remis à l'eau: détails biologiques enregistrés.
+Remis à l'eau, marqué (et échantillonné): Poisson capturé et remis à l'eau: détails biologiques enregistrés et le poisson a été marqué.
+Cicatrice, étiquette perdue, remis à l'eau: Poisson recapturé et relâché : la présence de cicatrices indique que le poisson a été marqué/étiqueté précédemment ; l'étiquette a été perdue.
+Inconnu: 
+</t>
   </si>
   <si>
     <t>life_stage__stade_de_vie</t>
@@ -286,6 +300,27 @@
   </si>
   <si>
     <t>Identifiant unique du spécimen</t>
+  </si>
+  <si>
+    <t>ITIS TSN</t>
+  </si>
+  <si>
+    <t>wms</t>
+  </si>
+  <si>
+    <t>The unique identifier for the Integrated Taxonomic Information System (ITIS)</t>
+  </si>
+  <si>
+    <t>L'identifiant unique du système intégré d'information taxonomique (SITI)</t>
+  </si>
+  <si>
+    <t>CGNDB</t>
+  </si>
+  <si>
+    <t>reference number in the Canadian Geographical Names Database (CGNDB)</t>
+  </si>
+  <si>
+    <t>numéro de référence dans la Base de données toponymiques du Canada (BDTC)</t>
   </si>
 </sst>
 </file>
@@ -352,12 +387,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:C29" totalsRowShown="0">
-  <autoFilter ref="A3:C29"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:D31" totalsRowShown="0">
+  <autoFilter ref="A3:D31"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="NAME__NOM"/>
-    <tableColumn id="2" name="DESCRIPTION_EN"/>
-    <tableColumn id="3" name="DESCRIPTION_FR"/>
+    <tableColumn id="2" name="DOCUMENT"/>
+    <tableColumn id="3" name="DESCRIPTION_EN"/>
+    <tableColumn id="4" name="DESCRIPTION_FR"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -648,23 +684,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="67.85546875" customWidth="1"/>
-    <col min="2" max="2" width="110.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="110.7109375" customWidth="1"/>
+    <col min="4" max="4" width="110.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -674,291 +711,400 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>22</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>28</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>31</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>34</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>37</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>40</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>43</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>46</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>49</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>52</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>55</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>58</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>62</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>65</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>68</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>69</v>
+        <v>6</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>71</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>72</v>
+        <v>6</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>74</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>77</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating datasets for restigouche RST data in order to exclude all sites that are not from `Kedgwick-RST`; removing geojson files (part III)
</commit_message>
<xml_diff>
--- a/17bda544 (restigouche RST)/rst_data_dictionary.xlsx
+++ b/17bda544 (restigouche RST)/rst_data_dictionary.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fishmand\Projects\fgp-datasets\17bda544 (restigouche RST)\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0AE9C6-9CF7-47BB-9665-E328962A3E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dict" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="82">
   <si>
     <t>Data Dictionary - dictionnaire des données</t>
   </si>
@@ -301,33 +307,12 @@
   <si>
     <t>Identifiant unique du spécimen</t>
   </si>
-  <si>
-    <t>ITIS TSN</t>
-  </si>
-  <si>
-    <t>wms</t>
-  </si>
-  <si>
-    <t>The unique identifier for the Integrated Taxonomic Information System (ITIS)</t>
-  </si>
-  <si>
-    <t>L'identifiant unique du système intégré d'information taxonomique (SITI)</t>
-  </si>
-  <si>
-    <t>CGNDB</t>
-  </si>
-  <si>
-    <t>reference number in the Canadian Geographical Names Database (CGNDB)</t>
-  </si>
-  <si>
-    <t>numéro de référence dans la Base de données toponymiques du Canada (BDTC)</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,26 +368,34 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:D31" totalsRowShown="0">
-  <autoFilter ref="A3:D31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A3:D29" totalsRowShown="0">
+  <autoFilter ref="A3:D29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="NAME__NOM"/>
-    <tableColumn id="2" name="DOCUMENT"/>
-    <tableColumn id="3" name="DESCRIPTION_EN"/>
-    <tableColumn id="4" name="DESCRIPTION_FR"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NAME__NOM"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="DOCUMENT"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="DESCRIPTION_EN"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="DESCRIPTION_FR"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -440,7 +433,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -474,6 +467,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -508,9 +502,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -683,25 +678,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:B31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="110.7109375" customWidth="1"/>
-    <col min="4" max="4" width="110.7109375" customWidth="1"/>
+    <col min="3" max="4" width="110.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -715,7 +711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -729,7 +725,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -743,7 +739,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -757,7 +753,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -771,7 +767,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -785,7 +781,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -799,7 +795,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -813,7 +809,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -827,7 +823,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>30</v>
       </c>
@@ -841,7 +837,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
@@ -855,7 +851,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -869,7 +865,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
@@ -883,7 +879,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>42</v>
       </c>
@@ -897,7 +893,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>45</v>
       </c>
@@ -911,7 +907,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" ht="375" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>48</v>
       </c>
@@ -925,7 +921,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
@@ -939,7 +935,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>54</v>
       </c>
@@ -953,7 +949,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>57</v>
       </c>
@@ -967,7 +963,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>60</v>
       </c>
@@ -981,7 +977,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>61</v>
       </c>
@@ -995,7 +991,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>64</v>
       </c>
@@ -1009,7 +1005,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>67</v>
       </c>
@@ -1023,7 +1019,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>70</v>
       </c>
@@ -1037,7 +1033,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>73</v>
       </c>
@@ -1051,7 +1047,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>76</v>
       </c>
@@ -1065,7 +1061,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>79</v>
       </c>
@@ -1077,34 +1073,6 @@
       </c>
       <c r="D29" s="2" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>